<commit_message>
massive amount of changes - havent committed in a long time
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/390 reddit star system 1/395 revised reddit star system 1.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/390 reddit star system 1/395 revised reddit star system 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/390 reddit star system 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1FA34C-C8B9-C246-844E-7299B255F574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DE713D-CC8A-FE41-8901-3175BAC0E2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{E25848C3-FC7E-AE48-8103-5EAA195D4710}"/>
   </bookViews>
@@ -676,8 +676,8 @@
   <dimension ref="D1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>